<commit_message>
Added Record to ScenaroFile - Akshat Branch
</commit_message>
<xml_diff>
--- a/ScenarioFile.xlsx
+++ b/ScenarioFile.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aksha\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My_Experiments\CheckProject\MainRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{838287AA-264C-41FF-96D3-5B6033E3C47D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{699AAFF2-7C0F-4FD5-B49A-AF6CDF22856A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2910" yWindow="3750" windowWidth="21600" windowHeight="11385" xr2:uid="{E33DE75D-066E-483F-BD60-7DE7F75AD8AD}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
   <si>
     <t>NAME</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>HIMANSHU</t>
+  </si>
+  <si>
+    <t>ABHISHEK</t>
   </si>
 </sst>
 </file>
@@ -401,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41B117A1-E7CB-487D-BE39-2CE6DAE428F8}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,6 +456,17 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added record - Gattoo Branch
</commit_message>
<xml_diff>
--- a/ScenarioFile.xlsx
+++ b/ScenarioFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My_Experiments\CheckProject\MainRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{699AAFF2-7C0F-4FD5-B49A-AF6CDF22856A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{882F3B33-FD4A-4D59-8AA7-677B513F4094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2910" yWindow="3750" windowWidth="21600" windowHeight="11385" xr2:uid="{E33DE75D-066E-483F-BD60-7DE7F75AD8AD}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
   <si>
     <t>NAME</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>ABHISHEK</t>
+  </si>
+  <si>
+    <t>GATTOO</t>
   </si>
 </sst>
 </file>
@@ -404,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41B117A1-E7CB-487D-BE39-2CE6DAE428F8}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,6 +470,17 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added record - Akki branch
</commit_message>
<xml_diff>
--- a/ScenarioFile.xlsx
+++ b/ScenarioFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My_Experiments\CheckProject\MainRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{699AAFF2-7C0F-4FD5-B49A-AF6CDF22856A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDA47D7-87C8-4CD1-A78D-88A79A762150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2910" yWindow="3750" windowWidth="21600" windowHeight="11385" xr2:uid="{E33DE75D-066E-483F-BD60-7DE7F75AD8AD}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
   <si>
     <t>NAME</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>ABHISHEK</t>
+  </si>
+  <si>
+    <t>Naman</t>
   </si>
 </sst>
 </file>
@@ -404,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41B117A1-E7CB-487D-BE39-2CE6DAE428F8}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,6 +470,17 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>